<commit_message>
Sript to generate inserts via excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prapo\Documents\MerdasUni\2023 - 1st Semester\BDDAD\LAPR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96257D3-D7E1-4066-8E02-A6D48DB39794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE373A83-AE7D-4006-95A3-0CAD96C96921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantas" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="236">
   <si>
     <t>Espécie</t>
   </si>
@@ -264,9 +264,6 @@
     <t>SUMMER RED</t>
   </si>
   <si>
-    <t>WELL'SPUR DELICIOUS</t>
-  </si>
-  <si>
     <t>NOIVA</t>
   </si>
   <si>
@@ -726,9 +723,6 @@
     <t>S. Cosme</t>
   </si>
   <si>
-    <t>Fevereiro a abril, agosto a outubro</t>
-  </si>
-  <si>
     <t>90 dias</t>
   </si>
   <si>
@@ -748,6 +742,15 @@
   </si>
   <si>
     <t>Perc.4</t>
+  </si>
+  <si>
+    <t>WELLSPUR DELICIOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agosto a outubro</t>
+  </si>
+  <si>
+    <t>Fevereiro a abril</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA74F46-7FB7-481B-9DAE-CE325D568C4A}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2353,7 @@
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -2373,7 +2376,7 @@
         <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -2396,7 +2399,7 @@
         <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -2419,7 +2422,7 @@
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -2442,7 +2445,7 @@
         <v>48</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -2465,7 +2468,7 @@
         <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -2488,7 +2491,7 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2511,7 +2514,7 @@
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -2534,7 +2537,7 @@
         <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -2557,7 +2560,7 @@
         <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -2580,7 +2583,7 @@
         <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -2603,7 +2606,7 @@
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -2626,7 +2629,7 @@
         <v>48</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
@@ -2649,7 +2652,7 @@
         <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -2672,7 +2675,7 @@
         <v>48</v>
       </c>
       <c r="C67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
@@ -2695,7 +2698,7 @@
         <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -2718,7 +2721,7 @@
         <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -2735,13 +2738,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" t="s">
         <v>90</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>91</v>
-      </c>
-      <c r="C70" t="s">
-        <v>92</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -2749,13 +2752,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71" t="s">
         <v>90</v>
       </c>
-      <c r="B71" t="s">
-        <v>91</v>
-      </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -2763,13 +2766,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" t="s">
         <v>90</v>
       </c>
-      <c r="B72" t="s">
-        <v>91</v>
-      </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -2777,13 +2780,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" t="s">
         <v>90</v>
       </c>
-      <c r="B73" t="s">
-        <v>91</v>
-      </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -2791,365 +2794,368 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" t="s">
         <v>96</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>97</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>98</v>
       </c>
-      <c r="D74" t="s">
+      <c r="H74" t="s">
         <v>99</v>
-      </c>
-      <c r="H74" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" t="s">
         <v>96</v>
       </c>
-      <c r="B75" t="s">
-        <v>97</v>
-      </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D75" t="s">
+        <v>98</v>
+      </c>
+      <c r="H75" t="s">
         <v>99</v>
-      </c>
-      <c r="H75" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" t="s">
         <v>96</v>
       </c>
-      <c r="B76" t="s">
-        <v>97</v>
-      </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D76" t="s">
+        <v>98</v>
+      </c>
+      <c r="H76" t="s">
         <v>99</v>
-      </c>
-      <c r="H76" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" t="s">
         <v>96</v>
       </c>
-      <c r="B77" t="s">
-        <v>97</v>
-      </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D77" t="s">
+        <v>98</v>
+      </c>
+      <c r="H77" t="s">
         <v>99</v>
-      </c>
-      <c r="H77" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" t="s">
         <v>96</v>
       </c>
-      <c r="B78" t="s">
-        <v>97</v>
-      </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D78" t="s">
+        <v>98</v>
+      </c>
+      <c r="H78" t="s">
         <v>99</v>
-      </c>
-      <c r="H78" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" t="s">
         <v>96</v>
       </c>
-      <c r="B79" t="s">
-        <v>97</v>
-      </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D79" t="s">
+        <v>98</v>
+      </c>
+      <c r="H79" t="s">
         <v>99</v>
-      </c>
-      <c r="H79" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" t="s">
         <v>96</v>
       </c>
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D80" t="s">
+        <v>98</v>
+      </c>
+      <c r="H80" t="s">
         <v>99</v>
-      </c>
-      <c r="H80" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" t="s">
         <v>107</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>108</v>
       </c>
-      <c r="C81" t="s">
-        <v>109</v>
-      </c>
       <c r="D81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" t="s">
         <v>110</v>
       </c>
-      <c r="B82" t="s">
-        <v>108</v>
-      </c>
-      <c r="C82" t="s">
-        <v>111</v>
-      </c>
       <c r="D82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
         <v>112</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>113</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>98</v>
+      </c>
+      <c r="E83" t="s">
         <v>114</v>
       </c>
-      <c r="D83" t="s">
-        <v>99</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="H83" t="s">
         <v>115</v>
-      </c>
-      <c r="H83" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" t="s">
         <v>112</v>
       </c>
-      <c r="B84" t="s">
-        <v>113</v>
-      </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E84" t="s">
+        <v>114</v>
+      </c>
+      <c r="H84" t="s">
         <v>115</v>
-      </c>
-      <c r="H84" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>117</v>
+      </c>
+      <c r="B85" t="s">
         <v>118</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>119</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>98</v>
+      </c>
+      <c r="E85" t="s">
         <v>120</v>
       </c>
-      <c r="D85" t="s">
-        <v>99</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="H85" t="s">
         <v>121</v>
-      </c>
-      <c r="H85" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86" t="s">
         <v>123</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>124</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" t="s">
         <v>125</v>
-      </c>
-      <c r="D86" t="s">
-        <v>11</v>
-      </c>
-      <c r="H86" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" t="s">
         <v>123</v>
       </c>
-      <c r="B87" t="s">
-        <v>124</v>
-      </c>
       <c r="C87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
       </c>
       <c r="H87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" t="s">
         <v>123</v>
       </c>
-      <c r="B88" t="s">
-        <v>124</v>
-      </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
       <c r="H88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" t="s">
         <v>123</v>
       </c>
-      <c r="B89" t="s">
-        <v>124</v>
-      </c>
       <c r="C89" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
       </c>
       <c r="H89" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" t="s">
         <v>123</v>
       </c>
-      <c r="B90" t="s">
-        <v>124</v>
-      </c>
       <c r="C90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
       </c>
       <c r="H90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" t="s">
         <v>123</v>
       </c>
-      <c r="B91" t="s">
-        <v>124</v>
-      </c>
       <c r="C91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
       <c r="H91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>122</v>
+      </c>
+      <c r="B92" t="s">
         <v>123</v>
       </c>
-      <c r="B92" t="s">
-        <v>124</v>
-      </c>
       <c r="C92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D92" t="s">
         <v>11</v>
       </c>
       <c r="H92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>122</v>
+      </c>
+      <c r="B93" t="s">
         <v>123</v>
       </c>
-      <c r="B93" t="s">
-        <v>124</v>
-      </c>
       <c r="C93" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
       </c>
       <c r="H93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>223</v>
+      </c>
+      <c r="B94" t="s">
         <v>224</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>225</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
+        <v>98</v>
+      </c>
+      <c r="E94" t="s">
+        <v>235</v>
+      </c>
+      <c r="F94" t="s">
+        <v>234</v>
+      </c>
+      <c r="H94" t="s">
         <v>226</v>
-      </c>
-      <c r="D94" t="s">
-        <v>99</v>
-      </c>
-      <c r="E94" t="s">
-        <v>227</v>
-      </c>
-      <c r="H94" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3163,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8BE3C6-089F-4A17-B7E6-182E6A73873F}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3183,63 +3189,63 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>137</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>138</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H1" t="s">
         <v>139</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" t="s">
         <v>231</v>
       </c>
-      <c r="H1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" t="s">
         <v>232</v>
-      </c>
-      <c r="J1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" t="s">
-        <v>233</v>
-      </c>
-      <c r="L1" t="s">
-        <v>142</v>
-      </c>
-      <c r="M1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>145</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>146</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>147</v>
-      </c>
-      <c r="F2" t="s">
-        <v>148</v>
       </c>
       <c r="G2" s="5">
         <v>0.2</v>
@@ -3247,22 +3253,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
         <v>149</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" t="s">
         <v>150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" t="s">
-        <v>151</v>
       </c>
       <c r="G3" s="5">
         <v>0.8</v>
@@ -3270,34 +3276,34 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
         <v>152</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>153</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>154</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>155</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>156</v>
-      </c>
-      <c r="F4" t="s">
-        <v>157</v>
       </c>
       <c r="G4" s="5">
         <v>0.249</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" s="3">
         <v>0.06</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="4">
         <v>0.17599999999999999</v>
@@ -3305,28 +3311,28 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>154</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>155</v>
       </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
       <c r="F5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="5">
         <v>0.151</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" s="4">
         <v>0.20799999999999999</v>
@@ -3334,40 +3340,40 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" t="s">
         <v>160</v>
       </c>
-      <c r="B6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" t="s">
-        <v>161</v>
-      </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" s="5">
         <v>0.09</v>
       </c>
       <c r="H6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="4">
         <v>0.124</v>
       </c>
       <c r="J6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K6" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="L6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M6" s="3">
         <v>0.01</v>
@@ -3375,28 +3381,28 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" t="s">
         <v>164</v>
       </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" t="s">
-        <v>165</v>
-      </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G7" s="5">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I7" s="3">
         <v>0.13</v>
@@ -3404,28 +3410,28 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
         <v>166</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" t="s">
         <v>167</v>
       </c>
-      <c r="C8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>168</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>169</v>
-      </c>
-      <c r="F8" t="s">
-        <v>170</v>
       </c>
       <c r="G8" s="5">
         <v>0.88200000000000001</v>
       </c>
       <c r="H8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I8" s="4">
         <v>1.9E-2</v>
@@ -3433,34 +3439,34 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" t="s">
         <v>172</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>167</v>
       </c>
-      <c r="C9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>168</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>169</v>
-      </c>
-      <c r="F9" t="s">
-        <v>170</v>
       </c>
       <c r="G9" s="5">
         <v>0.71699999999999997</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I9" s="4">
         <v>0.14799999999999999</v>
       </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K9" s="4">
         <v>7.9000000000000001E-2</v>
@@ -3476,7 +3482,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,19 +3493,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3507,16 +3513,16 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>179</v>
       </c>
       <c r="D2">
         <v>1.2</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3524,16 +3530,16 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3541,16 +3547,16 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4">
         <v>1.5</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3558,16 +3564,16 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5">
         <v>0.8</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3575,16 +3581,16 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,16 +3598,16 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D7">
         <v>0.3</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3609,16 +3615,16 @@
         <v>201</v>
       </c>
       <c r="B8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" t="s">
         <v>185</v>
-      </c>
-      <c r="C8" t="s">
-        <v>186</v>
       </c>
       <c r="D8">
         <v>600</v>
       </c>
       <c r="E8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3626,16 +3632,16 @@
         <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D9">
         <v>800</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3643,16 +3649,16 @@
         <v>203</v>
       </c>
       <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
         <v>189</v>
-      </c>
-      <c r="C10" t="s">
-        <v>190</v>
       </c>
       <c r="D10">
         <v>900</v>
       </c>
       <c r="E10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3660,10 +3666,10 @@
         <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3671,16 +3677,16 @@
         <v>301</v>
       </c>
       <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" t="s">
         <v>192</v>
-      </c>
-      <c r="C12" t="s">
-        <v>193</v>
       </c>
       <c r="D12">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3694,7 +3700,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,28 +3713,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
         <v>195</v>
       </c>
-      <c r="D1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>196</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>197</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>198</v>
-      </c>
-      <c r="H1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3736,10 +3742,10 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
         <v>200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>201</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -3751,7 +3757,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3759,10 +3765,10 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -3774,7 +3780,7 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3782,10 +3788,10 @@
         <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3797,7 +3803,7 @@
         <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3805,10 +3811,10 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -3820,7 +3826,7 @@
         <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3828,10 +3834,10 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -3843,7 +3849,7 @@
         <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3851,10 +3857,10 @@
         <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -3866,7 +3872,7 @@
         <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3874,13 +3880,13 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="1">
         <v>44114</v>
@@ -3892,7 +3898,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3900,13 +3906,13 @@
         <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="1">
         <v>44296</v>
@@ -3918,7 +3924,7 @@
         <v>0.9</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3926,13 +3932,13 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1">
         <v>44301</v>
@@ -3944,7 +3950,7 @@
         <v>0.9</v>
       </c>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3952,13 +3958,13 @@
         <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1">
         <v>44472</v>
@@ -3970,7 +3976,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3978,13 +3984,13 @@
         <v>106</v>
       </c>
       <c r="B12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" t="s">
         <v>221</v>
       </c>
-      <c r="C12" t="s">
-        <v>222</v>
-      </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="1">
         <v>43871</v>
@@ -3996,7 +4002,7 @@
         <v>0.15</v>
       </c>
       <c r="H12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4004,13 +4010,13 @@
         <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="1">
         <v>43984</v>
@@ -4022,7 +4028,7 @@
         <v>0.1</v>
       </c>
       <c r="H13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4030,13 +4036,13 @@
         <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="1">
         <v>44094</v>
@@ -4048,7 +4054,7 @@
         <v>0.2</v>
       </c>
       <c r="H14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4056,13 +4062,13 @@
         <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" s="1">
         <v>44237</v>
@@ -4074,7 +4080,7 @@
         <v>0.15</v>
       </c>
       <c r="H15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4082,13 +4088,13 @@
         <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1">
         <v>44349</v>
@@ -4100,7 +4106,7 @@
         <v>0.1</v>
       </c>
       <c r="H16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4108,13 +4114,13 @@
         <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1">
         <v>44459</v>
@@ -4126,7 +4132,7 @@
         <v>0.2</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4144,7 +4150,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+      <selection activeCell="I38" sqref="I38:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4161,31 +4167,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4193,13 +4199,13 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" t="s">
         <v>200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E2" t="s">
-        <v>201</v>
       </c>
       <c r="F2" s="1">
         <v>42649</v>
@@ -4208,7 +4214,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4216,13 +4222,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F3" s="1">
         <v>42653</v>
@@ -4231,7 +4237,7 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4239,13 +4245,13 @@
         <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" s="1">
         <v>42742</v>
@@ -4254,7 +4260,7 @@
         <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4262,13 +4268,13 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F5" s="1">
         <v>42743</v>
@@ -4277,7 +4283,7 @@
         <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4285,13 +4291,13 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F6" s="1">
         <v>42743</v>
@@ -4300,7 +4306,7 @@
         <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4308,10 +4314,10 @@
         <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
         <v>48</v>
@@ -4323,7 +4329,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4331,10 +4337,10 @@
         <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
@@ -4346,7 +4352,7 @@
         <v>3.5</v>
       </c>
       <c r="H8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4354,10 +4360,10 @@
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -4369,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4377,13 +4383,13 @@
         <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F10" s="1">
         <v>43043</v>
@@ -4392,7 +4398,7 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4400,13 +4406,13 @@
         <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F11" s="1">
         <v>43043</v>
@@ -4415,7 +4421,7 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4423,16 +4429,16 @@
         <v>102</v>
       </c>
       <c r="B12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" t="s">
         <v>200</v>
-      </c>
-      <c r="C12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" t="s">
-        <v>201</v>
       </c>
       <c r="F12" s="1">
         <v>43079</v>
@@ -4441,10 +4447,10 @@
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4452,16 +4458,16 @@
         <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F13" s="1">
         <v>43079</v>
@@ -4470,10 +4476,10 @@
         <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4481,10 +4487,10 @@
         <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" t="s">
         <v>48</v>
@@ -4496,7 +4502,7 @@
         <v>3.5</v>
       </c>
       <c r="H14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4504,10 +4510,10 @@
         <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" t="s">
         <v>48</v>
@@ -4519,7 +4525,7 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4527,10 +4533,10 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" t="s">
         <v>48</v>
@@ -4542,7 +4548,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4550,10 +4556,10 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s">
         <v>48</v>
@@ -4565,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4573,13 +4579,13 @@
         <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F18" s="1">
         <v>43421</v>
@@ -4588,7 +4594,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -4596,13 +4602,13 @@
         <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="1">
         <v>43421</v>
@@ -4611,7 +4617,7 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4619,13 +4625,13 @@
         <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="1">
         <v>43444</v>
@@ -4634,7 +4640,7 @@
         <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4642,10 +4648,10 @@
         <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E21" t="s">
         <v>48</v>
@@ -4657,7 +4663,7 @@
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4665,10 +4671,10 @@
         <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" t="s">
         <v>48</v>
@@ -4680,7 +4686,7 @@
         <v>4.5</v>
       </c>
       <c r="H22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4688,13 +4694,13 @@
         <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F23" s="1">
         <v>43784</v>
@@ -4703,7 +4709,7 @@
         <v>30</v>
       </c>
       <c r="H23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4711,13 +4717,13 @@
         <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F24" s="1">
         <v>43784</v>
@@ -4726,7 +4732,7 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4734,13 +4740,13 @@
         <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F25" s="1">
         <v>43956</v>
@@ -4749,7 +4755,7 @@
         <v>2200</v>
       </c>
       <c r="H25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4757,13 +4763,13 @@
         <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F26" s="1">
         <v>43966</v>
@@ -4772,7 +4778,7 @@
         <v>1400</v>
       </c>
       <c r="H26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4780,13 +4786,13 @@
         <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F27" s="1">
         <v>43984</v>
@@ -4795,7 +4801,7 @@
         <v>0.6</v>
       </c>
       <c r="H27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -4803,13 +4809,13 @@
         <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F28" s="1">
         <v>44071</v>
@@ -4818,7 +4824,7 @@
         <v>600</v>
       </c>
       <c r="H28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4826,13 +4832,13 @@
         <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F29" s="1">
         <v>44081</v>
@@ -4841,7 +4847,7 @@
         <v>1800</v>
       </c>
       <c r="H29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4849,13 +4855,13 @@
         <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F30" s="1">
         <v>44094</v>
@@ -4864,7 +4870,7 @@
         <v>0.6</v>
       </c>
       <c r="H30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4872,13 +4878,13 @@
         <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="1">
         <v>44114</v>
@@ -4887,7 +4893,7 @@
         <v>36</v>
       </c>
       <c r="H31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4895,13 +4901,13 @@
         <v>106</v>
       </c>
       <c r="B32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" t="s">
         <v>221</v>
-      </c>
-      <c r="C32" t="s">
-        <v>215</v>
-      </c>
-      <c r="E32" t="s">
-        <v>222</v>
       </c>
       <c r="F32" s="1">
         <v>44114</v>
@@ -4910,7 +4916,7 @@
         <v>0.9</v>
       </c>
       <c r="H32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4918,13 +4924,13 @@
         <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F33" s="1">
         <v>44145</v>
@@ -4933,7 +4939,7 @@
         <v>30</v>
       </c>
       <c r="H33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4941,13 +4947,13 @@
         <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F34" s="1">
         <v>44145</v>
@@ -4956,7 +4962,7 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4964,13 +4970,13 @@
         <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F35" s="1">
         <v>44150</v>
@@ -4979,7 +4985,7 @@
         <v>600</v>
       </c>
       <c r="H35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4987,13 +4993,13 @@
         <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F36" s="1">
         <v>44170</v>
@@ -5002,7 +5008,7 @@
         <v>70</v>
       </c>
       <c r="H36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -5010,13 +5016,13 @@
         <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F37" s="1">
         <v>44170</v>
@@ -5025,7 +5031,7 @@
         <v>50</v>
       </c>
       <c r="H37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -5033,16 +5039,16 @@
         <v>102</v>
       </c>
       <c r="B38" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38" t="s">
+        <v>228</v>
+      </c>
+      <c r="E38" t="s">
         <v>200</v>
-      </c>
-      <c r="C38" t="s">
-        <v>217</v>
-      </c>
-      <c r="D38" t="s">
-        <v>230</v>
-      </c>
-      <c r="E38" t="s">
-        <v>201</v>
       </c>
       <c r="F38" s="1">
         <v>44175</v>
@@ -5051,10 +5057,10 @@
         <v>10</v>
       </c>
       <c r="H38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -5062,16 +5068,16 @@
         <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D39" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F39" s="1">
         <v>44175</v>
@@ -5080,10 +5086,10 @@
         <v>7</v>
       </c>
       <c r="H39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -5091,13 +5097,13 @@
         <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F40" s="1">
         <v>44180</v>
@@ -5106,7 +5112,7 @@
         <v>40</v>
       </c>
       <c r="H40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -5114,13 +5120,13 @@
         <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F41" s="1">
         <v>44180</v>
@@ -5129,7 +5135,7 @@
         <v>60</v>
       </c>
       <c r="H41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5137,13 +5143,13 @@
         <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F42" s="1">
         <v>44183</v>
@@ -5152,7 +5158,7 @@
         <v>2500</v>
       </c>
       <c r="H42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -5160,13 +5166,13 @@
         <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F43" s="1">
         <v>44200</v>
@@ -5175,7 +5181,7 @@
         <v>2900</v>
       </c>
       <c r="H43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -5183,13 +5189,13 @@
         <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F44" s="1">
         <v>44285</v>
@@ -5200,13 +5206,13 @@
         <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F45" s="1">
         <v>44301</v>
@@ -5215,7 +5221,7 @@
         <v>30</v>
       </c>
       <c r="H45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -5223,13 +5229,13 @@
         <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D46" t="s">
         <v>217</v>
-      </c>
-      <c r="D46" t="s">
-        <v>218</v>
       </c>
       <c r="E46" t="s">
         <v>48</v>
@@ -5241,10 +5247,10 @@
         <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5252,13 +5258,13 @@
         <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F47" s="1">
         <v>44321</v>
@@ -5267,7 +5273,7 @@
         <v>2200</v>
       </c>
       <c r="H47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5275,13 +5281,13 @@
         <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F48" s="1">
         <v>44331</v>
@@ -5290,7 +5296,7 @@
         <v>1400</v>
       </c>
       <c r="H48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5298,13 +5304,13 @@
         <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F49" s="1">
         <v>44349</v>
@@ -5313,7 +5319,7 @@
         <v>0.6</v>
       </c>
       <c r="H49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -5321,10 +5327,10 @@
         <v>104</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E50" t="s">
         <v>48</v>
@@ -5336,7 +5342,7 @@
         <v>5</v>
       </c>
       <c r="H50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5344,13 +5350,13 @@
         <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F51" s="1">
         <v>44429</v>
@@ -5359,7 +5365,7 @@
         <v>3300</v>
       </c>
       <c r="H51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -5367,13 +5373,13 @@
         <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F52" s="1">
         <v>44432</v>
@@ -5382,7 +5388,7 @@
         <v>900</v>
       </c>
       <c r="H52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -5390,13 +5396,13 @@
         <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F53" s="1">
         <v>44436</v>
@@ -5405,7 +5411,7 @@
         <v>600</v>
       </c>
       <c r="H53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5413,13 +5419,13 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F54" s="1">
         <v>44444</v>
@@ -5428,7 +5434,7 @@
         <v>800</v>
       </c>
       <c r="H54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5436,13 +5442,13 @@
         <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F55" s="1">
         <v>44446</v>
@@ -5451,7 +5457,7 @@
         <v>1800</v>
       </c>
       <c r="H55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5459,13 +5465,13 @@
         <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F56" s="1">
         <v>44451</v>
@@ -5474,7 +5480,7 @@
         <v>800</v>
       </c>
       <c r="H56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -5482,13 +5488,13 @@
         <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E57" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F57" s="1">
         <v>44459</v>
@@ -5497,7 +5503,7 @@
         <v>0.6</v>
       </c>
       <c r="H57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5505,13 +5511,13 @@
         <v>104</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F58" s="1">
         <v>44462</v>
@@ -5520,7 +5526,7 @@
         <v>1200</v>
       </c>
       <c r="H58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -5528,13 +5534,13 @@
         <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F59" s="1">
         <v>44472</v>
@@ -5548,13 +5554,13 @@
         <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C60" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F60" s="1">
         <v>44479</v>
@@ -5563,7 +5569,7 @@
         <v>0.9</v>
       </c>
       <c r="H60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -5571,13 +5577,13 @@
         <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F61" s="1">
         <v>44481</v>
@@ -5586,7 +5592,7 @@
         <v>950</v>
       </c>
       <c r="H61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -5594,13 +5600,13 @@
         <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F62" s="1">
         <v>44503</v>
@@ -5609,7 +5615,7 @@
         <v>750</v>
       </c>
       <c r="H62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -5617,13 +5623,13 @@
         <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F63" s="1">
         <v>44515</v>
@@ -5632,7 +5638,7 @@
         <v>600</v>
       </c>
       <c r="H63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -5640,13 +5646,13 @@
         <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F64" s="1">
         <v>44517</v>
@@ -5655,7 +5661,7 @@
         <v>30</v>
       </c>
       <c r="H64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5663,13 +5669,13 @@
         <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="E65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F65" s="1">
         <v>44517</v>
@@ -5678,7 +5684,7 @@
         <v>20</v>
       </c>
       <c r="H65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -5686,13 +5692,13 @@
         <v>104</v>
       </c>
       <c r="B66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F66" s="1">
         <v>44528</v>
@@ -5701,7 +5707,7 @@
         <v>70</v>
       </c>
       <c r="H66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5709,13 +5715,13 @@
         <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="E67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F67" s="1">
         <v>44533</v>
@@ -5724,7 +5730,7 @@
         <v>90</v>
       </c>
       <c r="H67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5732,13 +5738,13 @@
         <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F68" s="1">
         <v>44548</v>
@@ -5747,7 +5753,7 @@
         <v>60</v>
       </c>
       <c r="H68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -5755,13 +5761,13 @@
         <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F69" s="1">
         <v>44548</v>
@@ -5770,7 +5776,7 @@
         <v>2500</v>
       </c>
       <c r="H69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5778,13 +5784,13 @@
         <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F70" s="1">
         <v>44565</v>
@@ -5793,7 +5799,7 @@
         <v>2900</v>
       </c>
       <c r="H70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5801,13 +5807,13 @@
         <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E71" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F71" s="1">
         <v>44656</v>
@@ -5818,13 +5824,13 @@
         <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F72" s="1">
         <v>44661</v>
@@ -5833,7 +5839,7 @@
         <v>30</v>
       </c>
       <c r="H72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -5841,13 +5847,13 @@
         <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" t="s">
         <v>217</v>
-      </c>
-      <c r="D73" t="s">
-        <v>218</v>
       </c>
       <c r="E73" t="s">
         <v>48</v>
@@ -5859,10 +5865,10 @@
         <v>10</v>
       </c>
       <c r="H73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -5870,13 +5876,13 @@
         <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F74" s="1">
         <v>44785</v>
@@ -5885,7 +5891,7 @@
         <v>3500</v>
       </c>
       <c r="H74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -5893,13 +5899,13 @@
         <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C75" t="s">
         <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F75" s="1">
         <v>44793</v>
@@ -5908,7 +5914,7 @@
         <v>950</v>
       </c>
       <c r="H75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -5916,13 +5922,13 @@
         <v>104</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F76" s="1">
         <v>44811</v>
@@ -5931,7 +5937,7 @@
         <v>830</v>
       </c>
       <c r="H76" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5939,13 +5945,13 @@
         <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F77" s="1">
         <v>44815</v>
@@ -5954,7 +5960,7 @@
         <v>750</v>
       </c>
       <c r="H77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5962,13 +5968,13 @@
         <v>104</v>
       </c>
       <c r="B78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F78" s="1">
         <v>44824</v>
@@ -5977,7 +5983,7 @@
         <v>1150</v>
       </c>
       <c r="H78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -5985,13 +5991,13 @@
         <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
       </c>
       <c r="E79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F79" s="1">
         <v>44851</v>
@@ -6000,7 +6006,7 @@
         <v>850</v>
       </c>
       <c r="H79" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -6008,13 +6014,13 @@
         <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F80" s="1">
         <v>44871</v>
@@ -6023,7 +6029,7 @@
         <v>900</v>
       </c>
       <c r="H80" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -6031,13 +6037,13 @@
         <v>102</v>
       </c>
       <c r="B81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
       </c>
       <c r="E81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F81" s="1">
         <v>44875</v>
@@ -6046,7 +6052,7 @@
         <v>30</v>
       </c>
       <c r="H81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -6054,13 +6060,13 @@
         <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
       <c r="E82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F82" s="1">
         <v>44875</v>
@@ -6069,7 +6075,7 @@
         <v>20</v>
       </c>
       <c r="H82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -6077,13 +6083,13 @@
         <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F83" s="1">
         <v>44899</v>
@@ -6092,7 +6098,7 @@
         <v>70</v>
       </c>
       <c r="H83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -6100,13 +6106,13 @@
         <v>104</v>
       </c>
       <c r="B84" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
       </c>
       <c r="E84" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F84" s="1">
         <v>44902</v>
@@ -6115,7 +6121,7 @@
         <v>90</v>
       </c>
       <c r="H84" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -6123,13 +6129,13 @@
         <v>104</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C85" t="s">
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F85" s="1">
         <v>44938</v>
@@ -6138,7 +6144,7 @@
         <v>60</v>
       </c>
       <c r="H85" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>